<commit_message>
finalna verzia článku spolu s finálnou podobou tabulky nástrojov
</commit_message>
<xml_diff>
--- a/tabulka_nastrojov.xlsx
+++ b/tabulka_nastrojov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonukus/Desktop/MIP_clanok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31270E55-5100-4A4A-A963-E57EC820BBE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AFA816-512B-4347-83A3-850250A3655A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{EA0E737B-D5F2-2249-9B1D-7E9A38313190}"/>
   </bookViews>
@@ -99,15 +99,6 @@
     <t xml:space="preserve">C# </t>
   </si>
   <si>
-    <t>Modely tried (Class)</t>
-  </si>
-  <si>
-    <t>Modely balíčkov (Package)</t>
-  </si>
-  <si>
-    <t>Sekvenčné modely (Sequence)</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -115,6 +106,15 @@
   </si>
   <si>
     <t>UML Diagramy</t>
+  </si>
+  <si>
+    <t>Diagramy balíčkov (Package)</t>
+  </si>
+  <si>
+    <t>Diagramy tried (Class)</t>
+  </si>
+  <si>
+    <t>Sekvenčné diagramy (Sequence)</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="B3:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,7 +641,7 @@
     <col min="4" max="10" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -663,7 +663,7 @@
       <c r="J3" s="15"/>
       <c r="K3" s="16"/>
       <c r="L3" s="17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -696,13 +696,13 @@
         <v>13</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.25">
@@ -738,10 +738,10 @@
         <v>4</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N5" s="11">
         <v>0</v>
@@ -783,10 +783,10 @@
         <v>0</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="21" x14ac:dyDescent="0.25">
@@ -822,10 +822,10 @@
         <v>3</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N7" s="11">
         <v>0</v>
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N8" s="11">
         <v>0</v>
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N9" s="11">
         <v>0</v>
@@ -951,10 +951,10 @@
         <v>0</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="21" x14ac:dyDescent="0.25">
@@ -993,10 +993,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="21" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>